<commit_message>
A dynamic and scalable Excel tool
</commit_message>
<xml_diff>
--- a/Company Information.xlsx
+++ b/Company Information.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop_Backup_July2025\Excel-Based-Forecasting-Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0188788C-266F-4306-B78E-DE0CE86D0D09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB16CC0-6E45-45E8-B282-992CFF49280F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{3E9885B1-F401-4922-BB4D-BD7E0F03B686}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="5" activeTab="9" xr2:uid="{3E9885B1-F401-4922-BB4D-BD7E0F03B686}"/>
   </bookViews>
   <sheets>
     <sheet name="Input" sheetId="1" r:id="rId1"/>
@@ -22,14 +22,15 @@
     <sheet name="TopLicenses" sheetId="10" r:id="rId7"/>
     <sheet name="AllocationPlan" sheetId="5" r:id="rId8"/>
     <sheet name="ForecastPeriods" sheetId="6" r:id="rId9"/>
+    <sheet name="Dashboard" sheetId="11" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlcn.WorksheetConnection_AllocationPlanA1G1001" hidden="1">AllocationPlan!$A$1:$G$100</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="45" r:id="rId10"/>
-    <pivotCache cacheId="51" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId11"/>
+    <pivotCache cacheId="1" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,9 +82,10 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <metadataTypes count="1">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="2">
     <metadataType name="XLMDX" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
   <metadataStrings count="2">
     <s v="ThisWorkbookDataModel"/>
@@ -94,6 +96,20 @@
       <ms ns="1" c="0"/>
     </mdx>
   </mdxMetadata>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="2" v="0"/>
+    </bk>
+  </cellMetadata>
   <valueMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
@@ -103,7 +119,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="102">
   <si>
     <t>Data Category</t>
   </si>
@@ -388,13 +404,35 @@
   </si>
   <si>
     <t>Utilization Alert</t>
+  </si>
+  <si>
+    <t>Cost per Active User</t>
+  </si>
+  <si>
+    <t>Buffer (%)</t>
+  </si>
+  <si>
+    <t>Total Forecasted Cost</t>
+  </si>
+  <si>
+    <t>Total Allocated Licenses</t>
+  </si>
+  <si>
+    <t>Average Cost per Active User</t>
+  </si>
+  <si>
+    <t>Count of Over-Provisioned</t>
+  </si>
+  <si>
+    <t>Licenses Over $30/User</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -442,7 +480,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -473,13 +511,114 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="7" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="7" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -490,6 +629,2710 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Forecasted Cost by Business Unit</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllocationPlan!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Finance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT Support</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marketing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllocationPlan!$G$2:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1600</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2800</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>456</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-8C3D-4F89-9972-105E2BE71018}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="1653368431"/>
+        <c:axId val="1653369391"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1653368431"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1653369391"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1653369391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1653368431"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Buffer % by Business Unit</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllocationPlan!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Finance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT Support</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marketing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllocationPlan!$I$2:$I$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-5291-4ECB-B9DF-E596D45DFDCB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1950007391"/>
+        <c:axId val="1950005471"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1950007391"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1950005471"/>
+        <c:crossesAt val="0"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1950005471"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1950007391"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Cost per Active User</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>AllocationPlan!$A$2:$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>Finance</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>IT Support</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marketing</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>AllocationPlan!$H$2:$H$4</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00_);\("$"#,##0.00\)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>33.684210526315788</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>138.88888888888889</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.814814814814815</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C987-49F6-9FBD-7055260E0E51}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="182"/>
+        <c:axId val="1664871919"/>
+        <c:axId val="1664873359"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1664871919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1664873359"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1664873359"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.0_);\(&quot;$&quot;#,##0.0\)" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1664871919"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="12">
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>527050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>222250</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB7559CC-2B84-4FDA-9220-110EB2B5D2CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>539750</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{718908B0-322D-49D0-A27A-8C2856D5DEDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>330200</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>546100</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A0F0878-1F72-449D-8196-028023643E93}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -658,7 +3501,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C7E492A1-4A4F-4806-815C-F96596CD1989}" name="PivotTable1" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C7E492A1-4A4F-4806-815C-F96596CD1989}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C10" firstHeaderRow="0" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="5">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -762,7 +3605,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8C292A84-2EC7-4252-B03D-81ABCC145ABD}" name="PivotTable2" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8C292A84-2EC7-4252-B03D-81ABCC145ABD}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField axis="axisRow" showAll="0">
@@ -816,7 +3659,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{892E1DF9-B804-4CFA-916B-15789523FA83}" name="PivotTable3" cacheId="51" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{892E1DF9-B804-4CFA-916B-15789523FA83}" name="PivotTable3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -1207,36 +4050,32 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.6328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" bestFit="1" customWidth="1"/>
+    <col min="1" max="5" width="40.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:5" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="12" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1253,7 +4092,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1270,7 +4109,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1287,7 +4126,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1304,7 +4143,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -1321,7 +4160,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>29</v>
       </c>
@@ -1341,6 +4180,72 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6E56B63-C6A3-47D1-AFE9-36FCC4694BE8}">
+  <dimension ref="B2:C6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L17" sqref="L17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="17">
+        <f>SUM(AllocationPlan!G2:G1000)</f>
+        <v>4856</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="17">
+        <f>SUM(AllocationPlan!D2:D1000)</f>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="17" cm="1">
+        <f t="array" ref="C4">ROUND(AVERAGE(IF(ISNUMBER(AllocationPlan!H2:H1000), AllocationPlan!H2:H1000)), 2)</f>
+        <v>62.46</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="17">
+        <f>COUNTIF(AllocationPlan!I2:I1000,"&lt;5%")</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C6" s="17">
+        <f>COUNTIF(AllocationPlan!H2:H1000,"&gt;30")</f>
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1532,7 +4437,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1642,8 +4547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67214F81-4BD5-42ED-A311-4FFCB881FD36}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1681,6 +4586,10 @@
       <c r="D2" s="2">
         <v>95</v>
       </c>
+      <c r="E2" t="str">
+        <f>IF(D2&lt;70, "Underutilized", "OK")</f>
+        <v>OK</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
@@ -1695,6 +4604,10 @@
       <c r="D3" s="2">
         <v>60</v>
       </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E7" si="0">IF(D3&lt;70, "Underutilized", "OK")</f>
+        <v>Underutilized</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
@@ -1709,6 +4622,10 @@
       <c r="D4" s="2">
         <v>72</v>
       </c>
+      <c r="E4" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
@@ -1723,6 +4640,10 @@
       <c r="D5" s="2">
         <v>88</v>
       </c>
+      <c r="E5" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
@@ -1737,6 +4658,10 @@
       <c r="D6" s="2">
         <v>92</v>
       </c>
+      <c r="E6" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="20" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
@@ -1750,6 +4675,10 @@
       </c>
       <c r="D7" s="2">
         <v>81</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="0"/>
+        <v>OK</v>
       </c>
     </row>
   </sheetData>
@@ -1795,17 +4724,15 @@
       <c r="A4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>50</v>
       </c>
-      <c r="C5" s="12">
+      <c r="C5">
         <v>1600</v>
       </c>
     </row>
@@ -1813,17 +4740,15 @@
       <c r="A6" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>28</v>
       </c>
-      <c r="C7" s="12">
+      <c r="C7">
         <v>2800</v>
       </c>
     </row>
@@ -1831,17 +4756,15 @@
       <c r="A8" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="B9" s="12">
+      <c r="B9">
         <v>38</v>
       </c>
-      <c r="C9" s="12">
+      <c r="C9">
         <v>456</v>
       </c>
     </row>
@@ -1849,10 +4772,10 @@
       <c r="A10" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B10" s="12">
+      <c r="B10">
         <v>116</v>
       </c>
-      <c r="C10" s="12">
+      <c r="C10">
         <v>4856</v>
       </c>
     </row>
@@ -1866,7 +4789,7 @@
   <dimension ref="A3:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1887,7 +4810,7 @@
       <c r="A4" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>1600</v>
       </c>
     </row>
@@ -1895,7 +4818,7 @@
       <c r="A5" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>2800</v>
       </c>
     </row>
@@ -1903,7 +4826,7 @@
       <c r="A6" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>456</v>
       </c>
     </row>
@@ -1911,7 +4834,7 @@
       <c r="A7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>4856</v>
       </c>
     </row>
@@ -1946,7 +4869,7 @@
       <c r="A4" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="12">
+      <c r="B4">
         <v>2800</v>
       </c>
     </row>
@@ -1954,7 +4877,7 @@
       <c r="A5" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="12">
+      <c r="B5">
         <v>1600</v>
       </c>
     </row>
@@ -1962,7 +4885,7 @@
       <c r="A6" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="12">
+      <c r="B6">
         <v>456</v>
       </c>
     </row>
@@ -1970,7 +4893,7 @@
       <c r="A7" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="12">
+      <c r="B7">
         <v>4856</v>
       </c>
     </row>
@@ -1981,10 +4904,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A04849D-65A1-4646-8E21-460EE5CC0596}">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1992,9 +4915,11 @@
     <col min="1" max="5" width="20.6328125" customWidth="1"/>
     <col min="6" max="6" width="29.6328125" customWidth="1"/>
     <col min="7" max="7" width="30.6328125" customWidth="1"/>
+    <col min="8" max="8" width="20.6328125" style="14" customWidth="1"/>
+    <col min="9" max="9" width="20.6328125" style="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>65</v>
       </c>
@@ -2016,8 +4941,14 @@
       <c r="G1" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>68</v>
       </c>
@@ -2040,8 +4971,16 @@
         <f>D2 * _xlfn.XLOOKUP(B2, LicenseCatalog!A:A, LicenseCatalog!D:D)</f>
         <v>1600</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H2" s="14">
+        <f>IFERROR(G2 / (D2 * VLOOKUP(B2, UsageData!B:D, 3, FALSE) / 100), "N/A")</f>
+        <v>33.684210526315788</v>
+      </c>
+      <c r="I2" s="16">
+        <f>IFERROR((E2 - D2) / E2, "N/A")</f>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>70</v>
       </c>
@@ -2064,8 +5003,16 @@
         <f>D3 * _xlfn.XLOOKUP(B3, LicenseCatalog!A:A, LicenseCatalog!D:D)</f>
         <v>2800</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="14">
+        <f>IFERROR(G3 / (D3 * VLOOKUP(B3, UsageData!B:D, 3, FALSE) / 100), "N/A")</f>
+        <v>138.88888888888889</v>
+      </c>
+      <c r="I3" s="16">
+        <f t="shared" ref="I3:I4" si="0">IFERROR((E3 - D3) / E3, "N/A")</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>72</v>
       </c>
@@ -2088,8 +5035,28 @@
         <f>D4 * _xlfn.XLOOKUP(B4, LicenseCatalog!A:A, LicenseCatalog!D:D)</f>
         <v>456</v>
       </c>
+      <c r="H4" s="14">
+        <f>IFERROR(G4 / (D4 * VLOOKUP(B4, UsageData!B:D, 3, FALSE) / 100), "N/A")</f>
+        <v>14.814814814814815</v>
+      </c>
+      <c r="I4" s="16">
+        <f t="shared" si="0"/>
+        <v>0.05</v>
+      </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="I2:I4">
+    <cfRule type="cellIs" priority="3" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="between">
+      <formula>0.05</formula>
+      <formula>0.15</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+      <formula>0.15</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>